<commit_message>
Add new static files
</commit_message>
<xml_diff>
--- a/static/files/RMI_Report_2020_Stock_Exchanges.xlsx
+++ b/static/files/RMI_Report_2020_Stock_Exchanges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gregoire.bellois\Seafile\RMI-ResearchTeam\RMI 2020\Contextual Information\Excel files for Website\Final versions for sharing with Antistatique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3677FE41-BA7A-48E2-A088-3483E97C285E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8B65AD-AAC6-43D3-8224-DE15592F4E44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="1935" windowWidth="28800" windowHeight="18525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RMI_Report_2020_Stock_Exchanges" sheetId="1" r:id="rId1"/>
@@ -840,6 +840,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C68" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:C68" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C68">
+    <sortCondition ref="A1:A68"/>
+  </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Company"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Stock Exchange"/>
@@ -1148,8 +1151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,10 +1178,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1186,10 +1189,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1197,10 +1200,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1208,10 +1211,10 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1219,10 +1222,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1230,10 +1233,10 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1241,10 +1244,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1274,10 +1277,10 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1285,10 +1288,10 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1296,10 +1299,10 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1307,10 +1310,10 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1329,10 +1332,10 @@
         <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1340,10 +1343,10 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1362,10 +1365,10 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1373,10 +1376,10 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1403,79 +1406,79 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1505,10 +1508,10 @@
         <v>51</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1516,10 +1519,10 @@
         <v>51</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1549,10 +1552,10 @@
         <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1560,10 +1563,10 @@
         <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1626,10 +1629,10 @@
         <v>62</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C43" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1637,10 +1640,10 @@
         <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1714,10 +1717,10 @@
         <v>69</v>
       </c>
       <c r="B51" t="s">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="C51" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1725,10 +1728,10 @@
         <v>69</v>
       </c>
       <c r="B52" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>71</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1736,10 +1739,10 @@
         <v>69</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C53" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1777,40 +1780,40 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C57" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B58" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C58" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B59" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C59" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B60" t="s">
         <v>12</v>
@@ -1821,24 +1824,24 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B61" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C61" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B62" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C62" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>